<commit_message>
Update 20 - extent reports 2.4 fixed
</commit_message>
<xml_diff>
--- a/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
+++ b/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75692F83-5EF9-4BCF-955F-B7F6C2539D81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C1F340-1C88-4B62-903D-5AE67B56EFE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suits" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>TestA</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>TC02</t>
+  </si>
+  <si>
+    <t>Test@12</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -259,6 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -650,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +830,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
@@ -834,8 +838,8 @@
       <c r="D14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
+      <c r="E14" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Update 20 - extent reports 3.0 with screen shot
</commit_message>
<xml_diff>
--- a/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
+++ b/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C1F340-1C88-4B62-903D-5AE67B56EFE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Suits" sheetId="2" r:id="rId1"/>
@@ -158,7 +157,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,16 +182,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -246,23 +245,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -543,107 +539,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="8"/>
+    <col min="1" max="1" width="28.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -651,232 +647,230 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="19.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="6">
         <v>90</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="6">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D14" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D15" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="E15" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D14" r:id="rId1"/>
+    <hyperlink ref="E14" r:id="rId2"/>
+    <hyperlink ref="D15" r:id="rId3"/>
+    <hyperlink ref="E15" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>

</xml_diff>

<commit_message>
Update 22 - Blood Glucose Tracker
</commit_message>
<xml_diff>
--- a/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
+++ b/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBDC894-57C1-4D71-ACC4-C3F72FE224E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA5E1B-1122-44D5-8D30-7AB18EE150BA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>TestA</t>
   </si>
@@ -140,9 +140,6 @@
     <t>LoginSuite</t>
   </si>
   <si>
-    <t>AsthmaTrackerSuite</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
@@ -159,6 +156,87 @@
   </si>
   <si>
     <t>Hello789@</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>Verify that, system does not allow to log BG without valid date</t>
+  </si>
+  <si>
+    <t>Verify that, system does not allow to log BG without BG value</t>
+  </si>
+  <si>
+    <t>Verify that, system does not allow to log BG with value more than 99</t>
+  </si>
+  <si>
+    <t>Verify that, system successfully logs BG with valid values</t>
+  </si>
+  <si>
+    <t>BloodGlucoseTest</t>
+  </si>
+  <si>
+    <t>BloodGlucoseSuite</t>
+  </si>
+  <si>
+    <t>BGLevel</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>10:10 PM</t>
+  </si>
+  <si>
+    <t>Date is required.</t>
+  </si>
+  <si>
+    <t>10/10/2010</t>
+  </si>
+  <si>
+    <t>Level must be less than or equal to 99.</t>
+  </si>
+  <si>
+    <t>Successfully Saved</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Level must be greater than zero.</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Verify that, system successfully logs BG with Current Date and Time</t>
   </si>
 </sst>
 </file>
@@ -252,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -269,6 +347,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -553,7 +638,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,16 +660,16 @@
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -658,10 +743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,7 +759,9 @@
     <col min="6" max="6" width="14.6640625" style="6" customWidth="1"/>
     <col min="7" max="7" width="16.44140625" style="6" customWidth="1"/>
     <col min="8" max="8" width="13.109375" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="6"/>
+    <col min="9" max="9" width="33.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -684,7 +771,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -751,7 +838,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>1</v>
@@ -813,7 +900,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>23</v>
@@ -833,7 +920,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>31</v>
@@ -853,7 +940,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>30</v>
@@ -873,7 +960,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>31</v>
@@ -882,14 +969,207 @@
         <v>35</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -899,8 +1179,18 @@
     <hyperlink ref="E15" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="D16" r:id="rId5" xr:uid="{88026155-06FA-421C-AFD5-94753D8AD3CE}"/>
     <hyperlink ref="E16" r:id="rId6" xr:uid="{068724A9-8C45-4689-B5FA-F9E7CCB8AE15}"/>
+    <hyperlink ref="D20" r:id="rId7" xr:uid="{2944CA42-75C3-4A7E-81D9-43D6FF0A9125}"/>
+    <hyperlink ref="E20" r:id="rId8" xr:uid="{A43868D3-74EA-4BFC-A57B-3F1585B4FF67}"/>
+    <hyperlink ref="D21" r:id="rId9" xr:uid="{442CC4CC-D7A2-471A-AB73-BB7BD0804DFF}"/>
+    <hyperlink ref="D22" r:id="rId10" xr:uid="{61B3E6B4-2B4F-47AB-B944-0E32D9A2F089}"/>
+    <hyperlink ref="D23" r:id="rId11" xr:uid="{0A7C6059-4061-4439-AC0C-2F26F3AEF16D}"/>
+    <hyperlink ref="D24" r:id="rId12" xr:uid="{BAA1FDC4-CED2-49F4-8F0B-EC9C12938384}"/>
+    <hyperlink ref="E21" r:id="rId13" xr:uid="{1C6BE1A7-1267-4505-A2FE-54CF23DC2AD4}"/>
+    <hyperlink ref="E22" r:id="rId14" xr:uid="{45A7C05C-C5D5-4ABA-AEE1-B77C9FB3A80F}"/>
+    <hyperlink ref="E23" r:id="rId15" xr:uid="{A849CC75-3419-435F-8DA7-9D6BA4792048}"/>
+    <hyperlink ref="E24" r:id="rId16" xr:uid="{0B241F65-E607-4E71-AC6C-C2B3ADB44C4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 23- bg profile
</commit_message>
<xml_diff>
--- a/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
+++ b/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA5E1B-1122-44D5-8D30-7AB18EE150BA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09105547-9830-4B08-AAAA-53B503B85D19}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>TestA</t>
   </si>
@@ -237,6 +237,15 @@
   </si>
   <si>
     <t>Verify that, system successfully logs BG with Current Date and Time</t>
+  </si>
+  <si>
+    <t>BloodGlucoseOnProfile</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>Verify that, system updates BG values on Profile page</t>
   </si>
 </sst>
 </file>
@@ -743,10 +752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B20" sqref="B20:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,7 +1026,7 @@
         <v>45</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>50</v>
@@ -1047,7 +1056,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>51</v>
@@ -1077,7 +1086,7 @@
         <v>47</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>52</v>
@@ -1107,7 +1116,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>71</v>
@@ -1136,7 +1145,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>53</v>
@@ -1170,6 +1179,63 @@
       <c r="F25" s="17"/>
       <c r="G25" s="11"/>
       <c r="H25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1189,8 +1255,10 @@
     <hyperlink ref="E22" r:id="rId14" xr:uid="{45A7C05C-C5D5-4ABA-AEE1-B77C9FB3A80F}"/>
     <hyperlink ref="E23" r:id="rId15" xr:uid="{A849CC75-3419-435F-8DA7-9D6BA4792048}"/>
     <hyperlink ref="E24" r:id="rId16" xr:uid="{0B241F65-E607-4E71-AC6C-C2B3ADB44C4F}"/>
+    <hyperlink ref="D28" r:id="rId17" xr:uid="{FEE19AE8-376D-48D2-B872-BDF3DDB292C0}"/>
+    <hyperlink ref="E28" r:id="rId18" xr:uid="{E3FEB062-74A8-4B8B-83D4-798807E5EAB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update - Articles & Downloads
</commit_message>
<xml_diff>
--- a/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
+++ b/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D45B3DB-8789-494C-A112-FB3FB022F55F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8851937C-6A23-42AD-9889-A6DA60A8D06C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14517" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14539" uniqueCount="945">
   <si>
     <t>LoginTest</t>
   </si>
@@ -3016,6 +3016,21 @@
   </si>
   <si>
     <t>videos</t>
+  </si>
+  <si>
+    <t>TC54</t>
+  </si>
+  <si>
+    <t>TC55</t>
+  </si>
+  <si>
+    <t>articles</t>
+  </si>
+  <si>
+    <t>downloads</t>
+  </si>
+  <si>
+    <t>TC56</t>
   </si>
 </sst>
 </file>
@@ -3639,10 +3654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:ID115"/>
+  <dimension ref="A1:ID123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115:E115"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -43024,7 +43039,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="108" spans="1:238" ht="72">
+    <row r="108" spans="1:238" ht="57.6">
       <c r="A108" s="25" t="s">
         <v>17</v>
       </c>
@@ -45912,10 +45927,10 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="35" t="s">
-        <v>931</v>
+        <v>940</v>
       </c>
       <c r="B115" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C115" s="33" t="s">
         <v>938</v>
@@ -45924,6 +45939,84 @@
         <v>5</v>
       </c>
       <c r="E115" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="34" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E118" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="35" t="s">
+        <v>941</v>
+      </c>
+      <c r="B119" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C119" s="33" t="s">
+        <v>938</v>
+      </c>
+      <c r="D119" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E119" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="34" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E122" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="35" t="s">
+        <v>944</v>
+      </c>
+      <c r="B123" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" s="33" t="s">
+        <v>938</v>
+      </c>
+      <c r="D123" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E123" s="19" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update in the select current date function
</commit_message>
<xml_diff>
--- a/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
+++ b/meschino/src/main/java/com/qa/meschino/testdata/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB3C40B-B734-40A3-B736-BC850F47235D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0578FA38-A092-4FEF-B881-9DB94C0CDC9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58560" yWindow="1140" windowWidth="21360" windowHeight="12285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suits" sheetId="2" r:id="rId1"/>
@@ -3211,7 +3211,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3274,6 +3274,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -3559,7 +3560,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3590,7 +3591,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3613,8 +3614,8 @@
       <c r="A6" s="4" t="s">
         <v>945</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3678,8 +3679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:ID127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -4133,8 +4134,8 @@
       <c r="A12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>8</v>
+      <c r="B12" s="36" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>43</v>
@@ -45952,7 +45953,7 @@
         <v>940</v>
       </c>
       <c r="B115" s="35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C115" s="33" t="s">
         <v>938</v>
@@ -45991,7 +45992,7 @@
         <v>941</v>
       </c>
       <c r="B119" s="35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C119" s="33" t="s">
         <v>948</v>
@@ -46030,7 +46031,7 @@
         <v>944</v>
       </c>
       <c r="B123" s="35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C123" s="33" t="s">
         <v>949</v>
@@ -46069,7 +46070,7 @@
         <v>947</v>
       </c>
       <c r="B127" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C127" s="33" t="s">
         <v>950</v>

</xml_diff>